<commit_message>
Implemented deployed new smart contract
</commit_message>
<xml_diff>
--- a/weekend-project-2/Transactions-report.xlsx
+++ b/weekend-project-2/Transactions-report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikos\Desktop\SolidityBootcamp\Encode-Solidity-Bootcamp-Weekend-Projects\weekend-project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D7163A-BC71-4194-A5BB-CDEDDB2C47A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD7B20B-6048-4461-B816-43A9320000FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24285" yWindow="2805" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7245" yWindow="1440" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Nikos</t>
   </si>
@@ -118,18 +118,35 @@
   </si>
   <si>
     <t>Contract deployment with 2 proposals (array parameter) coffee[0] tea[1]</t>
+  </si>
+  <si>
+    <t>0x325fde66e12f6b44a18a1512e9cc138f5fa705a931fb6b6274d7ff8630ac3202</t>
+  </si>
+  <si>
+    <t>giveRightToVote / address / 	0xE3A9a11232f4D52786CA61f56bB7Fb01b00C80cd</t>
+  </si>
+  <si>
+    <t>Nikos give rights to to Eniola so he can vote</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -178,9 +195,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -202,6 +219,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -495,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,10 +584,10 @@
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -639,7 +659,7 @@
       <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="11" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -649,7 +669,26 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="17" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="9" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>